<commit_message>
update: read and write permission
</commit_message>
<xml_diff>
--- a/data/cn_inflation_rate_to_be_calculated_2023.06.01-2024.06.01.xlsx
+++ b/data/cn_inflation_rate_to_be_calculated_2023.06.01-2024.06.01.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/winter/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/biboy/research/new_babe/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E9456BE4-CEA3-0D4D-8A85-C6A3D0DA1C97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B218CCA4-4A8B-5A49-BE35-BCF7E5F0F554}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="10220" windowWidth="15120" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="我的数列" sheetId="1" r:id="rId1"/>
@@ -30,14 +30,14 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="176" formatCode="0.000"/>
-    <numFmt numFmtId="177" formatCode="mm/yyyy"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="mm/yyyy"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -45,7 +45,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -54,13 +54,13 @@
       <i/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -88,13 +88,13 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -402,9 +402,9 @@
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:38">
+    <row r="1" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -446,7 +446,7 @@
       <c r="AK1" s="3"/>
       <c r="AL1" s="3"/>
     </row>
-    <row r="2" spans="1:38">
+    <row r="2" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
         <v>45047</v>
       </c>
@@ -470,7 +470,7 @@
       <c r="V2" s="1"/>
       <c r="W2" s="1"/>
     </row>
-    <row r="3" spans="1:38">
+    <row r="3" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
         <v>45078</v>
       </c>
@@ -494,7 +494,7 @@
       <c r="V3" s="1"/>
       <c r="W3" s="1"/>
     </row>
-    <row r="4" spans="1:38">
+    <row r="4" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
         <v>45108</v>
       </c>
@@ -518,7 +518,7 @@
       <c r="V4" s="1"/>
       <c r="W4" s="1"/>
     </row>
-    <row r="5" spans="1:38">
+    <row r="5" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
         <v>45139</v>
       </c>
@@ -542,7 +542,7 @@
       <c r="V5" s="1"/>
       <c r="W5" s="1"/>
     </row>
-    <row r="6" spans="1:38">
+    <row r="6" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
         <v>45170</v>
       </c>
@@ -566,7 +566,7 @@
       <c r="V6" s="1"/>
       <c r="W6" s="1"/>
     </row>
-    <row r="7" spans="1:38">
+    <row r="7" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
         <v>45200</v>
       </c>
@@ -590,7 +590,7 @@
       <c r="V7" s="1"/>
       <c r="W7" s="1"/>
     </row>
-    <row r="8" spans="1:38">
+    <row r="8" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
         <v>45231</v>
       </c>
@@ -614,7 +614,7 @@
       <c r="V8" s="1"/>
       <c r="W8" s="1"/>
     </row>
-    <row r="9" spans="1:38">
+    <row r="9" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
         <v>45261</v>
       </c>
@@ -638,7 +638,7 @@
       <c r="V9" s="1"/>
       <c r="W9" s="1"/>
     </row>
-    <row r="10" spans="1:38">
+    <row r="10" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
         <v>45292</v>
       </c>
@@ -662,7 +662,7 @@
       <c r="V10" s="1"/>
       <c r="W10" s="1"/>
     </row>
-    <row r="11" spans="1:38">
+    <row r="11" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
         <v>45323</v>
       </c>
@@ -686,7 +686,7 @@
       <c r="V11" s="1"/>
       <c r="W11" s="1"/>
     </row>
-    <row r="12" spans="1:38">
+    <row r="12" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
         <v>45352</v>
       </c>
@@ -710,7 +710,7 @@
       <c r="V12" s="1"/>
       <c r="W12" s="1"/>
     </row>
-    <row r="13" spans="1:38">
+    <row r="13" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A13" s="4">
         <v>45383</v>
       </c>
@@ -734,7 +734,7 @@
       <c r="V13" s="1"/>
       <c r="W13" s="1"/>
     </row>
-    <row r="14" spans="1:38">
+    <row r="14" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A14" s="4">
         <v>45413</v>
       </c>
@@ -758,7 +758,7 @@
       <c r="V14" s="1"/>
       <c r="W14" s="1"/>
     </row>
-    <row r="15" spans="1:38">
+    <row r="15" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A15" s="4"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>

</xml_diff>